<commit_message>
V0.2, produces single sandwich,  st with prompt in expander
</commit_message>
<xml_diff>
--- a/Ramon Puls.xlsx
+++ b/Ramon Puls.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Feedback\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\piotr.janczewski\Desktop\genAI\Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D108BF1C-C478-439F-B343-AB5DAE32A39E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEEA652B-9431-4E7B-A5C0-DF1E22A6F3E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,9 +45,6 @@
 Enter your Well.Better.Next. self-reflection and/or add your priorities context here</t>
   </si>
   <si>
-    <t>From Recognize || Unique Accenture Moments || Accenture achievements || Hello,   On behalf of AXA Health project Leadership, I would like to thank you for all commitment and time you spend working with us on the account which led us to the end of development of release 1.   We all appreciate your involvement  and we would like to show our gratitude with this points recognition.   Keep up the good work!   Thank you, AXA Health Team || 02-Mar-23</t>
-  </si>
-  <si>
     <t>Employee's Photo (Sanjeev Vohra)
 Sanjeev Vohra</t>
   </si>
@@ -55,12 +52,6 @@
     <t>From Recognize || Custom Program || Team Awards || In a year where AI generated a 3D view of the protein universe, Dall-E 2 took AI image generation to the next level and even Kendrick Lamar used deepfakes in his music video. All of you were our AI heroes, creating true value for our clients and helping them keep up with this vast pace of change.   And it’s certainly been a year of growth for us. We defined our 8 capabilities and brought you the iAi to help you all push the limits of your potential. Across the network, we welcomed Bridge i2i, Tenbu and Ergo to bolster our data and AI capabilities, had nearly 10,000 new faces join our network and came out on top as a leader in analyst rankings.   None of this would be possible without you, our builders, creators, designers and masters of data and AI, you truly put the art in Artificial Intelligence.  So here is a small token to say thank you for all you have done. Congratulations on keeping some of the biggest companies across the globe at the top of their data and AI game. || 26-Aug-22</t>
   </si>
   <si>
-    <t>I have been working with Rafal for the past one year. Rafal showed incredible leadership instincts in all tasks. He has incredible knowledge in Azure and optimum solutions for every complex problem. He is very positive person I would love to develop those skills. Amazing work.</t>
-  </si>
-  <si>
-    <t>From Recognize || Custom Program || Team Awards || Rafal - Congratulations on finishing in the Top 10 for the iAi Holiday Hackathon. On behalf of our collective team, thanks for your efforts and for continuing to help make these hackathons so impactful. iAi Team || 12-Jan-22</t>
-  </si>
-  <si>
     <t>Anytime Feedback Given: on Ramon Puls from Sanjeev Vohra on 29.08.2022</t>
   </si>
   <si>
@@ -70,30 +61,39 @@
     <t>Dana Kalm</t>
   </si>
   <si>
-    <t>Dear Rafal, 
+    <t>Anytime Feedback Given: on Ramon Puls from Nathaniel Kaffle on 03.03.2023</t>
+  </si>
+  <si>
+    <t>Nathaniel Kaffle</t>
+  </si>
+  <si>
+    <t>Feedback Given: on Ramon Puls from Sashka Shrama on 08.07.2022</t>
+  </si>
+  <si>
+    <t>Employee's Photo (Sashka Shrama (On Leave))
+Sashka Shrama</t>
+  </si>
+  <si>
+    <t>Anytime Feedback Given: on Ramon Puls from Mona Lizar on 13.01.2022</t>
+  </si>
+  <si>
+    <t>Employee's Photo (Mona Lizar)
+Mona Lizar</t>
+  </si>
+  <si>
+    <t>From Recognize || Unique Accenture Moments || Accenture achievements || Hello,   On behalf of AXA Health project Leadership, I would like to thank you for all commitment and time you spend working with us on the account which led us to the end of development of release 1.   We all appreciate your involvement  and we would like to show our gratitude with this points recognition. You could be more punctual.   Keep up the good work!   Thank you, AXA Health Team || 02-Mar-23</t>
+  </si>
+  <si>
+    <t>Dear Ramon, 
 I would like to express my sincere appreciation for your exceptional qualities as a colleague. Your technical expertise is truly remarkable, and your willingness to assist others is greatly valued. Your profound understanding of our current project is evident and highly beneficial. At present, I believe you have surpassed all expectations, leaving no room for improvement. I extend my heartfelt gratitude for the invaluable help and insightful suggestions you have provided. 
 Thank you immensely for your continued support and contributions. 
 Best regards,Dana Kalm</t>
   </si>
   <si>
-    <t>Anytime Feedback Given: on Ramon Puls from Nathaniel Kaffle on 03.03.2023</t>
-  </si>
-  <si>
-    <t>Nathaniel Kaffle</t>
-  </si>
-  <si>
-    <t>Feedback Given: on Ramon Puls from Sashka Shrama on 08.07.2022</t>
-  </si>
-  <si>
-    <t>Employee's Photo (Sashka Shrama (On Leave))
-Sashka Shrama</t>
-  </si>
-  <si>
-    <t>Anytime Feedback Given: on Ramon Puls from Mona Lizar on 13.01.2022</t>
-  </si>
-  <si>
-    <t>Employee's Photo (Mona Lizar)
-Mona Lizar</t>
+    <t>I have been working with Ramon for the past one year. Ramon showed incredible leadership instincts in all tasks. He has incredible knowledge in Azure and optimum solutions for every complex problem. He is very positive person I would love to develop those skills. Amazing work.</t>
+  </si>
+  <si>
+    <t>From Recognize || Custom Program || Team Awards || Ramon - Congratulations on finishing in the Top 10 for the iAi Holiday Hackathon. On behalf of our collective team, thanks for your efforts and for continuing to help make these hackathons so impactful. iAi Team || 12-Jan-22</t>
   </si>
 </sst>
 </file>
@@ -490,12 +490,13 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="5" width="23" customWidth="1"/>
+    <col min="1" max="4" width="23" customWidth="1"/>
+    <col min="5" max="5" width="82.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -524,83 +525,83 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="331.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="140.25" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B3" s="4">
         <v>45119</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="255" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B4" s="4">
         <v>44988</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="153" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B5" s="4">
         <v>44802</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="165.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="140.25" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B6" s="4">
         <v>44750</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="165.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B7" s="4">
         <v>44574</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>